<commit_message>
Some code refactoring, increase reusability and customization
</commit_message>
<xml_diff>
--- a/data/chart_data.xlsx
+++ b/data/chart_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotr Kupczyk\Mój folder\Studia\Informatyczna techniczna\Praca magisterska\Model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2905AE3-55E1-42D7-9D02-73E7293392A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE5860F-1198-4324-84FD-BFF2A1679433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3A0DE45-8C9D-47FA-AE47-7FBC4D0760BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3A0DE45-8C9D-47FA-AE47-7FBC4D0760BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Training Data" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f>$R$2</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B2" s="2">
         <f>$S$2</f>
@@ -651,7 +651,7 @@
         <v>20</v>
       </c>
       <c r="R2" s="6">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -663,7 +663,7 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A66" si="0">$R$2</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B66" si="1">$S$2</f>
@@ -705,7 +705,7 @@
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" si="1"/>
@@ -747,7 +747,7 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="1"/>
@@ -789,7 +789,7 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="1"/>
@@ -831,7 +831,7 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="1"/>
@@ -873,7 +873,7 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="1"/>
@@ -915,7 +915,7 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="1"/>
@@ -957,7 +957,7 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="1"/>
@@ -999,7 +999,7 @@
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="1"/>
@@ -1041,7 +1041,7 @@
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="1"/>
@@ -1083,7 +1083,7 @@
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="1"/>
@@ -1125,7 +1125,7 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="1"/>
@@ -1167,7 +1167,7 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="1"/>
@@ -1209,7 +1209,7 @@
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="1"/>
@@ -1251,7 +1251,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="1"/>
@@ -1293,7 +1293,7 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="1"/>
@@ -1335,7 +1335,7 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="1"/>
@@ -1377,7 +1377,7 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="1"/>
@@ -1419,7 +1419,7 @@
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="1"/>
@@ -1461,7 +1461,7 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="1"/>
@@ -1503,7 +1503,7 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="1"/>
@@ -1545,7 +1545,7 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" si="1"/>
@@ -1587,7 +1587,7 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="1"/>
@@ -1629,7 +1629,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="1"/>
@@ -1671,7 +1671,7 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="1"/>
@@ -1713,7 +1713,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="1"/>
@@ -1755,7 +1755,7 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="1"/>
@@ -1797,7 +1797,7 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="1"/>
@@ -1839,7 +1839,7 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="1"/>
@@ -1881,7 +1881,7 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B32" s="2">
         <f t="shared" si="1"/>
@@ -1923,7 +1923,7 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B33" s="2">
         <f t="shared" si="1"/>
@@ -1965,7 +1965,7 @@
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B34" s="2">
         <f t="shared" si="1"/>
@@ -2007,7 +2007,7 @@
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B35" s="2">
         <f t="shared" si="1"/>
@@ -2049,7 +2049,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B36" s="2">
         <f t="shared" si="1"/>
@@ -2091,7 +2091,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B37" s="2">
         <f t="shared" si="1"/>
@@ -2133,7 +2133,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B38" s="2">
         <f t="shared" si="1"/>
@@ -2175,7 +2175,7 @@
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B39" s="2">
         <f t="shared" si="1"/>
@@ -2217,7 +2217,7 @@
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B40" s="2">
         <f t="shared" si="1"/>
@@ -2259,7 +2259,7 @@
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B41" s="2">
         <f t="shared" si="1"/>
@@ -2301,7 +2301,7 @@
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" si="1"/>
@@ -2343,7 +2343,7 @@
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B43" s="2">
         <f t="shared" si="1"/>
@@ -2385,7 +2385,7 @@
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B44" s="2">
         <f t="shared" si="1"/>
@@ -2427,7 +2427,7 @@
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B45" s="2">
         <f t="shared" si="1"/>
@@ -2469,7 +2469,7 @@
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B46" s="2">
         <f t="shared" si="1"/>
@@ -2511,7 +2511,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B47" s="2">
         <f t="shared" si="1"/>
@@ -2553,7 +2553,7 @@
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B48" s="2">
         <f t="shared" si="1"/>
@@ -2595,7 +2595,7 @@
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B49" s="2">
         <f t="shared" si="1"/>
@@ -2637,7 +2637,7 @@
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B50" s="2">
         <f t="shared" si="1"/>
@@ -2679,7 +2679,7 @@
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B51" s="2">
         <f t="shared" si="1"/>
@@ -2721,7 +2721,7 @@
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B52" s="2">
         <f t="shared" si="1"/>
@@ -2763,7 +2763,7 @@
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B53" s="2">
         <f t="shared" si="1"/>
@@ -2805,7 +2805,7 @@
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B54" s="2">
         <f t="shared" si="1"/>
@@ -2847,7 +2847,7 @@
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B55" s="2">
         <f t="shared" si="1"/>
@@ -2889,7 +2889,7 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B56" s="2">
         <f t="shared" si="1"/>
@@ -2931,7 +2931,7 @@
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B57" s="2">
         <f t="shared" si="1"/>
@@ -2973,7 +2973,7 @@
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B58" s="2">
         <f t="shared" si="1"/>
@@ -3015,7 +3015,7 @@
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B59" s="2">
         <f t="shared" si="1"/>
@@ -3057,7 +3057,7 @@
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B60" s="2">
         <f t="shared" si="1"/>
@@ -3099,7 +3099,7 @@
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B61" s="2">
         <f t="shared" si="1"/>
@@ -3141,7 +3141,7 @@
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B62" s="2">
         <f t="shared" si="1"/>
@@ -3183,7 +3183,7 @@
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B63" s="2">
         <f t="shared" si="1"/>
@@ -3225,7 +3225,7 @@
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B64" s="2">
         <f t="shared" si="1"/>
@@ -3267,7 +3267,7 @@
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B65" s="2">
         <f t="shared" si="1"/>
@@ -3309,7 +3309,7 @@
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B66" s="2">
         <f t="shared" si="1"/>
@@ -3351,7 +3351,7 @@
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <f t="shared" ref="A67:A130" si="10">$R$2</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B67" s="2">
         <f t="shared" ref="B67:B130" si="11">$S$2</f>
@@ -3393,7 +3393,7 @@
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B68" s="2">
         <f t="shared" si="11"/>
@@ -3435,7 +3435,7 @@
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B69" s="2">
         <f t="shared" si="11"/>
@@ -3477,7 +3477,7 @@
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B70" s="2">
         <f t="shared" si="11"/>
@@ -3519,7 +3519,7 @@
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B71" s="2">
         <f t="shared" si="11"/>
@@ -3561,7 +3561,7 @@
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B72" s="2">
         <f t="shared" si="11"/>
@@ -3603,7 +3603,7 @@
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B73" s="2">
         <f t="shared" si="11"/>
@@ -3645,7 +3645,7 @@
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B74" s="2">
         <f t="shared" si="11"/>
@@ -3687,7 +3687,7 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B75" s="2">
         <f t="shared" si="11"/>
@@ -3729,7 +3729,7 @@
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B76" s="2">
         <f t="shared" si="11"/>
@@ -3771,7 +3771,7 @@
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B77" s="2">
         <f t="shared" si="11"/>
@@ -3813,7 +3813,7 @@
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B78" s="2">
         <f t="shared" si="11"/>
@@ -3855,7 +3855,7 @@
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B79" s="2">
         <f t="shared" si="11"/>
@@ -3897,7 +3897,7 @@
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B80" s="2">
         <f t="shared" si="11"/>
@@ -3939,7 +3939,7 @@
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B81" s="2">
         <f t="shared" si="11"/>
@@ -3981,7 +3981,7 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B82" s="2">
         <f t="shared" si="11"/>
@@ -4023,7 +4023,7 @@
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B83" s="2">
         <f t="shared" si="11"/>
@@ -4065,7 +4065,7 @@
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B84" s="2">
         <f t="shared" si="11"/>
@@ -4107,7 +4107,7 @@
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B85" s="2">
         <f t="shared" si="11"/>
@@ -4149,7 +4149,7 @@
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B86" s="2">
         <f t="shared" si="11"/>
@@ -4191,7 +4191,7 @@
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B87" s="2">
         <f t="shared" si="11"/>
@@ -4233,7 +4233,7 @@
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B88" s="2">
         <f t="shared" si="11"/>
@@ -4275,7 +4275,7 @@
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B89" s="2">
         <f t="shared" si="11"/>
@@ -4317,7 +4317,7 @@
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B90" s="2">
         <f t="shared" si="11"/>
@@ -4359,7 +4359,7 @@
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B91" s="2">
         <f t="shared" si="11"/>
@@ -4401,7 +4401,7 @@
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B92" s="2">
         <f t="shared" si="11"/>
@@ -4443,7 +4443,7 @@
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B93" s="2">
         <f t="shared" si="11"/>
@@ -4485,7 +4485,7 @@
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B94" s="2">
         <f t="shared" si="11"/>
@@ -4527,7 +4527,7 @@
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B95" s="2">
         <f t="shared" si="11"/>
@@ -4569,7 +4569,7 @@
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B96" s="2">
         <f t="shared" si="11"/>
@@ -4611,7 +4611,7 @@
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B97" s="2">
         <f t="shared" si="11"/>
@@ -4653,7 +4653,7 @@
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B98" s="2">
         <f t="shared" si="11"/>
@@ -4695,7 +4695,7 @@
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B99" s="2">
         <f t="shared" si="11"/>
@@ -4737,7 +4737,7 @@
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B100" s="2">
         <f t="shared" si="11"/>
@@ -4779,7 +4779,7 @@
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B101" s="2">
         <f t="shared" si="11"/>
@@ -4821,7 +4821,7 @@
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B102" s="2">
         <f t="shared" si="11"/>
@@ -4863,7 +4863,7 @@
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B103" s="2">
         <f t="shared" si="11"/>
@@ -4905,7 +4905,7 @@
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B104" s="2">
         <f t="shared" si="11"/>
@@ -4947,7 +4947,7 @@
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B105" s="2">
         <f t="shared" si="11"/>
@@ -4989,7 +4989,7 @@
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B106" s="2">
         <f t="shared" si="11"/>
@@ -5031,7 +5031,7 @@
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B107" s="2">
         <f t="shared" si="11"/>
@@ -5073,7 +5073,7 @@
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B108" s="2">
         <f t="shared" si="11"/>
@@ -5115,7 +5115,7 @@
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B109" s="2">
         <f t="shared" si="11"/>
@@ -5157,7 +5157,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B110" s="2">
         <f t="shared" si="11"/>
@@ -5199,7 +5199,7 @@
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B111" s="2">
         <f t="shared" si="11"/>
@@ -5241,7 +5241,7 @@
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B112" s="2">
         <f t="shared" si="11"/>
@@ -5283,7 +5283,7 @@
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B113" s="2">
         <f t="shared" si="11"/>
@@ -5325,7 +5325,7 @@
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B114" s="2">
         <f t="shared" si="11"/>
@@ -5367,7 +5367,7 @@
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B115" s="2">
         <f t="shared" si="11"/>
@@ -5409,7 +5409,7 @@
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B116" s="2">
         <f t="shared" si="11"/>
@@ -5451,7 +5451,7 @@
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B117" s="2">
         <f t="shared" si="11"/>
@@ -5493,7 +5493,7 @@
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B118" s="2">
         <f t="shared" si="11"/>
@@ -5535,7 +5535,7 @@
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B119" s="2">
         <f t="shared" si="11"/>
@@ -5577,7 +5577,7 @@
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B120" s="2">
         <f t="shared" si="11"/>
@@ -5619,7 +5619,7 @@
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B121" s="2">
         <f t="shared" si="11"/>
@@ -5661,7 +5661,7 @@
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B122" s="2">
         <f t="shared" si="11"/>
@@ -5703,7 +5703,7 @@
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B123" s="2">
         <f t="shared" si="11"/>
@@ -5745,7 +5745,7 @@
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B124" s="2">
         <f t="shared" si="11"/>
@@ -5787,7 +5787,7 @@
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B125" s="2">
         <f t="shared" si="11"/>
@@ -5829,7 +5829,7 @@
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B126" s="2">
         <f t="shared" si="11"/>
@@ -5871,7 +5871,7 @@
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B127" s="2">
         <f t="shared" si="11"/>
@@ -5913,7 +5913,7 @@
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B128" s="2">
         <f t="shared" si="11"/>
@@ -5955,7 +5955,7 @@
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B129" s="2">
         <f t="shared" si="11"/>
@@ -5997,7 +5997,7 @@
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <f t="shared" si="10"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B130" s="2">
         <f t="shared" si="11"/>
@@ -6039,7 +6039,7 @@
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <f t="shared" ref="A131:A194" si="20">$R$2</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B131" s="2">
         <f t="shared" ref="B131:B194" si="21">$S$2</f>
@@ -6081,7 +6081,7 @@
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B132" s="2">
         <f t="shared" si="21"/>
@@ -6123,7 +6123,7 @@
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B133" s="2">
         <f t="shared" si="21"/>
@@ -6165,7 +6165,7 @@
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B134" s="2">
         <f t="shared" si="21"/>
@@ -6207,7 +6207,7 @@
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B135" s="2">
         <f t="shared" si="21"/>
@@ -6249,7 +6249,7 @@
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B136" s="2">
         <f t="shared" si="21"/>
@@ -6291,7 +6291,7 @@
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B137" s="2">
         <f t="shared" si="21"/>
@@ -6333,7 +6333,7 @@
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B138" s="2">
         <f t="shared" si="21"/>
@@ -6375,7 +6375,7 @@
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B139" s="2">
         <f t="shared" si="21"/>
@@ -6417,7 +6417,7 @@
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B140" s="2">
         <f t="shared" si="21"/>
@@ -6459,7 +6459,7 @@
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B141" s="2">
         <f t="shared" si="21"/>
@@ -6501,7 +6501,7 @@
     <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B142" s="2">
         <f t="shared" si="21"/>
@@ -6543,7 +6543,7 @@
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B143" s="2">
         <f t="shared" si="21"/>
@@ -6585,7 +6585,7 @@
     <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B144" s="2">
         <f t="shared" si="21"/>
@@ -6627,7 +6627,7 @@
     <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B145" s="2">
         <f t="shared" si="21"/>
@@ -6669,7 +6669,7 @@
     <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B146" s="2">
         <f t="shared" si="21"/>
@@ -6711,7 +6711,7 @@
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B147" s="2">
         <f t="shared" si="21"/>
@@ -6753,7 +6753,7 @@
     <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B148" s="2">
         <f t="shared" si="21"/>
@@ -6795,7 +6795,7 @@
     <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B149" s="2">
         <f t="shared" si="21"/>
@@ -6837,7 +6837,7 @@
     <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B150" s="2">
         <f t="shared" si="21"/>
@@ -6879,7 +6879,7 @@
     <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B151" s="2">
         <f t="shared" si="21"/>
@@ -6921,7 +6921,7 @@
     <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B152" s="2">
         <f t="shared" si="21"/>
@@ -6963,7 +6963,7 @@
     <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B153" s="2">
         <f t="shared" si="21"/>
@@ -7005,7 +7005,7 @@
     <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B154" s="2">
         <f t="shared" si="21"/>
@@ -7047,7 +7047,7 @@
     <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B155" s="2">
         <f t="shared" si="21"/>
@@ -7089,7 +7089,7 @@
     <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B156" s="2">
         <f t="shared" si="21"/>
@@ -7131,7 +7131,7 @@
     <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B157" s="2">
         <f t="shared" si="21"/>
@@ -7173,7 +7173,7 @@
     <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B158" s="2">
         <f t="shared" si="21"/>
@@ -7215,7 +7215,7 @@
     <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B159" s="2">
         <f t="shared" si="21"/>
@@ -7257,7 +7257,7 @@
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B160" s="2">
         <f t="shared" si="21"/>
@@ -7299,7 +7299,7 @@
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B161" s="2">
         <f t="shared" si="21"/>
@@ -7341,7 +7341,7 @@
     <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B162" s="2">
         <f t="shared" si="21"/>
@@ -7383,7 +7383,7 @@
     <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B163" s="2">
         <f t="shared" si="21"/>
@@ -7425,7 +7425,7 @@
     <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B164" s="2">
         <f t="shared" si="21"/>
@@ -7467,7 +7467,7 @@
     <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B165" s="2">
         <f t="shared" si="21"/>
@@ -7509,7 +7509,7 @@
     <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B166" s="2">
         <f t="shared" si="21"/>
@@ -7551,7 +7551,7 @@
     <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B167" s="2">
         <f t="shared" si="21"/>
@@ -7593,7 +7593,7 @@
     <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B168" s="2">
         <f t="shared" si="21"/>
@@ -7635,7 +7635,7 @@
     <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B169" s="2">
         <f t="shared" si="21"/>
@@ -7677,7 +7677,7 @@
     <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B170" s="2">
         <f t="shared" si="21"/>
@@ -7719,7 +7719,7 @@
     <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B171" s="2">
         <f t="shared" si="21"/>
@@ -7761,7 +7761,7 @@
     <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B172" s="2">
         <f t="shared" si="21"/>
@@ -7803,7 +7803,7 @@
     <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B173" s="2">
         <f t="shared" si="21"/>
@@ -7845,7 +7845,7 @@
     <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B174" s="2">
         <f t="shared" si="21"/>
@@ -7887,7 +7887,7 @@
     <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B175" s="2">
         <f t="shared" si="21"/>
@@ -7929,7 +7929,7 @@
     <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B176" s="2">
         <f t="shared" si="21"/>
@@ -7971,7 +7971,7 @@
     <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B177" s="2">
         <f t="shared" si="21"/>
@@ -8013,7 +8013,7 @@
     <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B178" s="2">
         <f t="shared" si="21"/>
@@ -8055,7 +8055,7 @@
     <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B179" s="2">
         <f t="shared" si="21"/>
@@ -8097,7 +8097,7 @@
     <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B180" s="2">
         <f t="shared" si="21"/>
@@ -8139,7 +8139,7 @@
     <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B181" s="2">
         <f t="shared" si="21"/>
@@ -8181,7 +8181,7 @@
     <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B182" s="2">
         <f t="shared" si="21"/>
@@ -8223,7 +8223,7 @@
     <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B183" s="2">
         <f t="shared" si="21"/>
@@ -8265,7 +8265,7 @@
     <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B184" s="2">
         <f t="shared" si="21"/>
@@ -8307,7 +8307,7 @@
     <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B185" s="2">
         <f t="shared" si="21"/>
@@ -8349,7 +8349,7 @@
     <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B186" s="2">
         <f t="shared" si="21"/>
@@ -8391,7 +8391,7 @@
     <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B187" s="2">
         <f t="shared" si="21"/>
@@ -8433,7 +8433,7 @@
     <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B188" s="2">
         <f t="shared" si="21"/>
@@ -8475,7 +8475,7 @@
     <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B189" s="2">
         <f t="shared" si="21"/>
@@ -8517,7 +8517,7 @@
     <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B190" s="2">
         <f t="shared" si="21"/>
@@ -8559,7 +8559,7 @@
     <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B191" s="2">
         <f t="shared" si="21"/>
@@ -8601,7 +8601,7 @@
     <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B192" s="2">
         <f t="shared" si="21"/>
@@ -8643,7 +8643,7 @@
     <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B193" s="2">
         <f t="shared" si="21"/>
@@ -8685,7 +8685,7 @@
     <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" s="2">
         <f t="shared" si="20"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B194" s="2">
         <f t="shared" si="21"/>
@@ -8727,7 +8727,7 @@
     <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" s="2">
         <f t="shared" ref="A195:A241" si="30">$R$2</f>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B195" s="2">
         <f t="shared" ref="B195:B241" si="31">$S$2</f>
@@ -8769,7 +8769,7 @@
     <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B196" s="2">
         <f t="shared" si="31"/>
@@ -8811,7 +8811,7 @@
     <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B197" s="2">
         <f t="shared" si="31"/>
@@ -8853,7 +8853,7 @@
     <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B198" s="2">
         <f t="shared" si="31"/>
@@ -8895,7 +8895,7 @@
     <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B199" s="2">
         <f t="shared" si="31"/>
@@ -8937,7 +8937,7 @@
     <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B200" s="2">
         <f t="shared" si="31"/>
@@ -8979,7 +8979,7 @@
     <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B201" s="2">
         <f t="shared" si="31"/>
@@ -9021,7 +9021,7 @@
     <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B202" s="2">
         <f t="shared" si="31"/>
@@ -9063,7 +9063,7 @@
     <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B203" s="2">
         <f t="shared" si="31"/>
@@ -9105,7 +9105,7 @@
     <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B204" s="2">
         <f t="shared" si="31"/>
@@ -9147,7 +9147,7 @@
     <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B205" s="2">
         <f t="shared" si="31"/>
@@ -9189,7 +9189,7 @@
     <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B206" s="2">
         <f t="shared" si="31"/>
@@ -9231,7 +9231,7 @@
     <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B207" s="2">
         <f t="shared" si="31"/>
@@ -9273,7 +9273,7 @@
     <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B208" s="2">
         <f t="shared" si="31"/>
@@ -9315,7 +9315,7 @@
     <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B209" s="2">
         <f t="shared" si="31"/>
@@ -9357,7 +9357,7 @@
     <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B210" s="2">
         <f t="shared" si="31"/>
@@ -9399,7 +9399,7 @@
     <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B211" s="2">
         <f t="shared" si="31"/>
@@ -9441,7 +9441,7 @@
     <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B212" s="2">
         <f t="shared" si="31"/>
@@ -9483,7 +9483,7 @@
     <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B213" s="2">
         <f t="shared" si="31"/>
@@ -9525,7 +9525,7 @@
     <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B214" s="2">
         <f t="shared" si="31"/>
@@ -9567,7 +9567,7 @@
     <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B215" s="2">
         <f t="shared" si="31"/>
@@ -9609,7 +9609,7 @@
     <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B216" s="2">
         <f t="shared" si="31"/>
@@ -9651,7 +9651,7 @@
     <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B217" s="2">
         <f t="shared" si="31"/>
@@ -9693,7 +9693,7 @@
     <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B218" s="2">
         <f t="shared" si="31"/>
@@ -9735,7 +9735,7 @@
     <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B219" s="2">
         <f t="shared" si="31"/>
@@ -9777,7 +9777,7 @@
     <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B220" s="2">
         <f t="shared" si="31"/>
@@ -9819,7 +9819,7 @@
     <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B221" s="2">
         <f t="shared" si="31"/>
@@ -9861,7 +9861,7 @@
     <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B222" s="2">
         <f t="shared" si="31"/>
@@ -9903,7 +9903,7 @@
     <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B223" s="2">
         <f t="shared" si="31"/>
@@ -9945,7 +9945,7 @@
     <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B224" s="2">
         <f t="shared" si="31"/>
@@ -9987,7 +9987,7 @@
     <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B225" s="2">
         <f t="shared" si="31"/>
@@ -10029,7 +10029,7 @@
     <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B226" s="2">
         <f t="shared" si="31"/>
@@ -10071,7 +10071,7 @@
     <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B227" s="2">
         <f t="shared" si="31"/>
@@ -10113,7 +10113,7 @@
     <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B228" s="2">
         <f t="shared" si="31"/>
@@ -10155,7 +10155,7 @@
     <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B229" s="2">
         <f t="shared" si="31"/>
@@ -10197,7 +10197,7 @@
     <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B230" s="2">
         <f t="shared" si="31"/>
@@ -10239,7 +10239,7 @@
     <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B231" s="2">
         <f t="shared" si="31"/>
@@ -10281,7 +10281,7 @@
     <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B232" s="2">
         <f t="shared" si="31"/>
@@ -10323,7 +10323,7 @@
     <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B233" s="2">
         <f t="shared" si="31"/>
@@ -10365,7 +10365,7 @@
     <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B234" s="2">
         <f t="shared" si="31"/>
@@ -10407,7 +10407,7 @@
     <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B235" s="2">
         <f t="shared" si="31"/>
@@ -10449,7 +10449,7 @@
     <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B236" s="2">
         <f t="shared" si="31"/>
@@ -10491,7 +10491,7 @@
     <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B237" s="2">
         <f t="shared" si="31"/>
@@ -10533,7 +10533,7 @@
     <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B238" s="2">
         <f t="shared" si="31"/>
@@ -10575,7 +10575,7 @@
     <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B239" s="2">
         <f t="shared" si="31"/>
@@ -10617,7 +10617,7 @@
     <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B240" s="2">
         <f t="shared" si="31"/>
@@ -10659,7 +10659,7 @@
     <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" s="2">
         <f t="shared" si="30"/>
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="B241" s="2">
         <f t="shared" si="31"/>

</xml_diff>